<commit_message>
-m "Added distance as a Design Variable"
</commit_message>
<xml_diff>
--- a/Decision_variables.xlsx
+++ b/Decision_variables.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23921"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mitprod.sharepoint.com/sites/EM.428MDOBiogasspring2021/Shared Documents/General/Assignment A2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niekjansenvanrensburg/Documents/MDO/Assignment_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{491E7ADF-991C-9441-B536-41DE1688ED44}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{AB3A845D-8415-4611-93BE-7C22936BC2D8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C4E8672-1D69-DE4C-8B28-EE3D1266B9DA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" xr2:uid="{3401D942-13D0-054C-9961-07B5F38F1A1A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="20740" windowHeight="11160" xr2:uid="{3401D942-13D0-054C-9961-07B5F38F1A1A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="DOE_options" sheetId="2" r:id="rId2"/>
     <sheet name="DOE_exp" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -261,7 +261,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -668,16 +668,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24EACC72-6EE8-9149-867A-69437CEA090E}">
   <dimension ref="A1:BE10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
-      <selection activeCell="AK1" sqref="AK1:AL1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="24" max="24" width="10.875" customWidth="1"/>
+    <col min="24" max="24" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" s="1" customFormat="1" ht="78.75">
+    <row r="1" spans="1:57" s="1" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -850,7 +850,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:57">
+    <row r="2" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -890,10 +890,10 @@
         <v>0.05</v>
       </c>
       <c r="M2" s="3">
+        <v>1</v>
+      </c>
+      <c r="N2" s="3">
         <v>0</v>
-      </c>
-      <c r="N2" s="3">
-        <v>1</v>
       </c>
       <c r="O2" s="3">
         <v>0</v>
@@ -912,10 +912,10 @@
         <v>0.03</v>
       </c>
       <c r="T2" s="3">
+        <v>1</v>
+      </c>
+      <c r="U2" s="3">
         <v>0</v>
-      </c>
-      <c r="U2" s="3">
-        <v>1</v>
       </c>
       <c r="V2" s="3">
         <v>0</v>
@@ -934,10 +934,10 @@
         <v>0.03</v>
       </c>
       <c r="AA2" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="3">
         <v>0</v>
-      </c>
-      <c r="AB2" s="3">
-        <v>1</v>
       </c>
       <c r="AC2" s="3">
         <v>0</v>
@@ -956,16 +956,16 @@
         <v>0.03</v>
       </c>
       <c r="AH2" s="3">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="3">
         <v>0</v>
-      </c>
-      <c r="AI2" s="3">
-        <v>1</v>
       </c>
       <c r="AJ2" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:57">
+    <row r="3" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -974,7 +974,7 @@
         <v>19.909999999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:57">
+    <row r="4" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -983,22 +983,22 @@
         <v>139.36999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:57">
+    <row r="5" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:57">
+    <row r="6" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:57">
+    <row r="7" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:57">
+    <row r="10" spans="1:57" x14ac:dyDescent="0.2">
       <c r="C10" s="6"/>
     </row>
   </sheetData>
@@ -1015,14 +1015,14 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>57</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>63</v>
       </c>
@@ -1062,7 +1062,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>63</v>
       </c>
@@ -1080,7 +1080,7 @@
       </c>
       <c r="F3" s="9"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>70</v>
       </c>
@@ -1112,19 +1112,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1274,19 +1271,45 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C000A07D-6CFC-4919-8B30-2A495D90C4E2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD1B1050-8496-49DB-876B-D84CEF4C6D2A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{667B1E25-096F-4EE8-B795-C44CED4F65E4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{667B1E25-096F-4EE8-B795-C44CED4F65E4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="50212d7f-d8f2-4c52-8864-549e1880ecad"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD1B1050-8496-49DB-876B-D84CEF4C6D2A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C000A07D-6CFC-4919-8B30-2A495D90C4E2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>